<commit_message>
Changed connector, started layout, save before reloading new netlist
</commit_message>
<xml_diff>
--- a/Hardware/Three_Phase_Inverter_Controller.xlsx
+++ b/Hardware/Three_Phase_Inverter_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="182">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">1206</t>
   </si>
   <si>
-    <t xml:space="preserve">CL31B475KBHVPNE</t>
+    <t xml:space="preserve">UMK316AB7475KL-T</t>
   </si>
   <si>
     <t xml:space="preserve">C43 </t>
@@ -136,43 +136,56 @@
     <t xml:space="preserve">POWER</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1” Header, 1x2, TH R</t>
+    <t xml:space="preserve">0.1” Header, 1x2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">A98333-ND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">J3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN/I2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1” Header, 2x8, TH R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM1224-08-ND</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
   </si>
   <si>
-    <t xml:space="preserve">J3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURRENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1” Header, 1x8, TH R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C</t>
+    <t xml:space="preserve">J4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART</t>
   </si>
   <si>
     <t xml:space="preserve">0.1” Header, 1x4, TH R</t>
   </si>
   <si>
-    <t xml:space="preserve">J5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPARE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UART</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J7 </t>
+    <t xml:space="preserve">SSQ-104-02-T-S-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J5</t>
   </si>
   <si>
     <t xml:space="preserve">USB_B</t>
@@ -181,7 +194,7 @@
     <t xml:space="preserve">Custom SMD USB B</t>
   </si>
   <si>
-    <t xml:space="preserve">J8 </t>
+    <t xml:space="preserve">J6</t>
   </si>
   <si>
     <t xml:space="preserve">ISP</t>
@@ -190,6 +203,9 @@
     <t xml:space="preserve">0.1” Header, 2x3, TH</t>
   </si>
   <si>
+    <t xml:space="preserve">Standard (owned)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Male</t>
   </si>
   <si>
@@ -253,6 +269,9 @@
     <t xml:space="preserve">SDR0604-680KL</t>
   </si>
   <si>
+    <t xml:space="preserve">SDR0604-680KLCT-ND </t>
+  </si>
+  <si>
     <t xml:space="preserve">Q1 Q2 Q3 Q4 Q5 Q6 </t>
   </si>
   <si>
@@ -439,15 +458,24 @@
     <t xml:space="preserve">5V_BUCK</t>
   </si>
   <si>
+    <t xml:space="preserve">TP8 TP9 TP10 TP11 … TP19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various</t>
+  </si>
+  <si>
     <t xml:space="preserve">TVS1 </t>
   </si>
   <si>
+    <t xml:space="preserve">PRTR5V0U2X,215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO-253-4</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRTR5V0U2X</t>
   </si>
   <si>
-    <t xml:space="preserve">TO-253-4</t>
-  </si>
-  <si>
     <t xml:space="preserve">U1 </t>
   </si>
   <si>
@@ -460,6 +488,9 @@
     <t xml:space="preserve">TPS22810DBVR</t>
   </si>
   <si>
+    <t xml:space="preserve">296-45297-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">U2 </t>
   </si>
   <si>
@@ -511,10 +542,10 @@
     <t xml:space="preserve">U6 </t>
   </si>
   <si>
-    <t xml:space="preserve">SN74LVC1G04-Q1</t>
-  </si>
-  <si>
     <t xml:space="preserve">SN74LVC1G04QDBVRQ1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-26588-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">U7 </t>
@@ -561,7 +592,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -623,6 +654,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -745,7 +782,7 @@
     <xf numFmtId="164" fontId="10" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -766,11 +803,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -867,10 +916,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,71 +1144,77 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="n">
         <f aca="false">B11*3</f>
         <v>3</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="F11" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="B12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="n">
         <f aca="false">B12*3</f>
-        <v>3</v>
-      </c>
-      <c r="D12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>39</v>
+      <c r="F12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="n">
         <f aca="false">B13*3</f>
         <v>3</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1</v>
@@ -1169,18 +1224,18 @@
         <v>3</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>62910416121</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1190,18 +1245,21 @@
         <v>3</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1211,18 +1269,21 @@
         <v>3</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>62910416121</v>
+        <v>59</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1232,19 +1293,21 @@
         <v>3</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="5"/>
       <c r="G17" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1254,21 +1317,21 @@
         <v>3</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1278,19 +1341,21 @@
         <v>3</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="G19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -1300,19 +1365,21 @@
         <v>3</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="G20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -1322,19 +1389,21 @@
         <v>3</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="G21" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -1344,41 +1413,43 @@
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="3" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B23*3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="3" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1</v>
@@ -1388,40 +1459,39 @@
         <v>3</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">B25*3</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="0" t="s">
-        <v>79</v>
+        <v>14</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -1431,60 +1501,60 @@
         <v>3</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">B27*3</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28*3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -1494,39 +1564,39 @@
         <v>3</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30*3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -1536,18 +1606,18 @@
         <v>3</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -1557,123 +1627,123 @@
         <v>3</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">B33*3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">B34*3</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">B35*3</f>
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">B36*3</f>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>109</v>
+        <v>25</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">B37*3</f>
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>14</v>
+        <v>122</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>123</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -1683,18 +1753,21 @@
         <v>3</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>119</v>
+        <v>126</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -1704,18 +1777,21 @@
         <v>3</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -1725,21 +1801,21 @@
         <v>3</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="E40" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>126</v>
+      <c r="F40" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -1749,21 +1825,21 @@
         <v>3</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>109</v>
+        <v>133</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>5019</v>
       </c>
       <c r="F41" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>126</v>
+      <c r="G41" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -1773,21 +1849,21 @@
         <v>3</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>109</v>
+        <v>135</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>5019</v>
       </c>
       <c r="F42" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>126</v>
+      <c r="G42" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -1797,21 +1873,21 @@
         <v>3</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>109</v>
+        <v>137</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>5019</v>
       </c>
       <c r="F43" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>126</v>
+      <c r="G43" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
@@ -1821,45 +1897,45 @@
         <v>3</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>109</v>
+        <v>139</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>5019</v>
       </c>
       <c r="F44" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>126</v>
+      <c r="G44" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C45" s="0" t="n">
+      <c r="A45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="C45" s="5" t="n">
         <f aca="false">B45*3</f>
-        <v>3</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="5" t="n">
         <v>5019</v>
       </c>
-      <c r="G45" s="6" t="s">
-        <v>126</v>
+      <c r="F45" s="5" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -1868,22 +1944,19 @@
         <f aca="false">B46*3</f>
         <v>3</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>138</v>
+      <c r="D46" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F46" s="3" t="n">
-        <v>5019</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>126</v>
+        <v>144</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1</v>
@@ -1893,18 +1966,21 @@
         <v>3</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>140</v>
+        <v>149</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -1914,18 +1990,18 @@
         <v>3</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
@@ -1935,18 +2011,18 @@
         <v>3</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -1956,63 +2032,66 @@
         <v>3</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">B51*3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" s="0" t="n">
         <f aca="false">B52*3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1</v>
@@ -2022,18 +2101,18 @@
         <v>3</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1</v>
@@ -2043,58 +2122,40 @@
         <v>3</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">B55*3</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <f aca="false">B56*3</f>
-        <v>9</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F56" s="0" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F11" r:id="rId1" display="A98333-ND"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Started layout. Minor adjustments to schematic to make layout easier.
</commit_message>
<xml_diff>
--- a/Hardware/Three_Phase_Inverter_Controller.xlsx
+++ b/Hardware/Three_Phase_Inverter_Controller.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="189">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -112,10 +112,22 @@
     <t xml:space="preserve">CL10C270JB8NNNC</t>
   </si>
   <si>
-    <t xml:space="preserve">D3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNJ167W8RRA</t>
+    <t xml:space="preserve">D3 D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SML-LX1206SUGC-TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SML-LX1206IC-TR</t>
   </si>
   <si>
     <t xml:space="preserve">D1 D2 D4 D5 D6 </t>
@@ -139,23 +151,7 @@
     <t xml:space="preserve">0.1” Header, 1x2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">A98333-ND</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t xml:space="preserve">A98333-ND </t>
   </si>
   <si>
     <t xml:space="preserve">J3 </t>
@@ -281,6 +277,15 @@
     <t xml:space="preserve">Already owned</t>
   </si>
   <si>
+    <t xml:space="preserve">Q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BSS806NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1 </t>
   </si>
   <si>
@@ -362,7 +367,7 @@
     <t xml:space="preserve">RC0603FR-0712KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R29 R30 </t>
+    <t xml:space="preserve">R29 R30 R39</t>
   </si>
   <si>
     <t xml:space="preserve">180R</t>
@@ -592,11 +597,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -614,57 +620,98 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -765,24 +812,56 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -803,23 +882,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -916,17 +983,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="91.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.45"/>
@@ -1106,136 +1173,136 @@
         <v>30</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9*3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">B10*3</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="n">
+      <c r="B11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <f aca="false">B11*3</f>
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="0" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">B12*3</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="5" t="n">
-        <f aca="false">B12*3</f>
+      <c r="C13" s="3" t="n">
+        <f aca="false">B13*3</f>
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">B13*3</f>
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="G13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="B14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="n">
         <f aca="false">B14*3</f>
         <v>3</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="3" t="n">
-        <v>62910416121</v>
+      <c r="F14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -1245,21 +1312,18 @@
         <v>3</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>56</v>
+      <c r="F15" s="3" t="n">
+        <v>62910416121</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
@@ -1269,21 +1333,21 @@
         <v>3</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -1293,21 +1357,21 @@
         <v>3</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>56</v>
+      <c r="G17" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1</v>
@@ -1317,21 +1381,21 @@
         <v>3</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>1</v>
@@ -1341,21 +1405,21 @@
         <v>3</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>55</v>
+      <c r="F19" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
@@ -1365,21 +1429,21 @@
         <v>3</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
@@ -1389,21 +1453,21 @@
         <v>3</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1</v>
@@ -1413,16 +1477,16 @@
         <v>3</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="8" t="s">
         <v>77</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,11 +1494,11 @@
         <v>78</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">B23*3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>79</v>
@@ -1442,48 +1506,51 @@
       <c r="E23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>80</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">B24*3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>83</v>
+        <v>18</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">B25*3</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>86</v>
@@ -1491,7 +1558,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>1</v>
@@ -1501,60 +1568,60 @@
         <v>3</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">B27*3</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">B28*3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1</v>
@@ -1564,39 +1631,39 @@
         <v>3</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">B30*3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -1606,18 +1673,18 @@
         <v>3</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -1627,31 +1694,31 @@
         <v>3</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">B33*3</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>111</v>
@@ -1662,17 +1729,17 @@
         <v>112</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">B34*3</f>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>113</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>114</v>
@@ -1683,59 +1750,59 @@
         <v>115</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">B35*3</f>
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>116</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>14</v>
+        <v>117</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">B36*3</f>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">B37*3</f>
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="0" t="s">
         <v>123</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>124</v>
@@ -1755,13 +1822,10 @@
       <c r="D38" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="3" t="n">
-        <v>5019</v>
-      </c>
-      <c r="F38" s="0" t="n">
-        <v>5019</v>
-      </c>
-      <c r="G38" s="8" t="s">
+      <c r="E38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="0" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1779,19 +1843,16 @@
       <c r="D39" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="E39" s="3" t="n">
-        <v>5019</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>5019</v>
-      </c>
-      <c r="G39" s="8" t="s">
-        <v>127</v>
+      <c r="E39" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -1801,21 +1862,21 @@
         <v>3</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E40" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="0" t="n">
         <v>5019</v>
       </c>
-      <c r="G40" s="8" t="s">
-        <v>127</v>
+      <c r="G40" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1</v>
@@ -1825,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>5019</v>
@@ -1833,13 +1894,13 @@
       <c r="F41" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G41" s="8" t="s">
-        <v>127</v>
+      <c r="G41" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -1849,7 +1910,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>5019</v>
@@ -1857,13 +1918,13 @@
       <c r="F42" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>127</v>
+      <c r="G42" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1</v>
@@ -1873,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>5019</v>
@@ -1881,13 +1942,13 @@
       <c r="F43" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G43" s="8" t="s">
-        <v>127</v>
+      <c r="G43" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1</v>
@@ -1897,7 +1958,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>5019</v>
@@ -1905,37 +1966,37 @@
       <c r="F44" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>127</v>
+      <c r="G44" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="C45" s="5" t="n">
+      <c r="A45" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="n">
         <f aca="false">B45*3</f>
-        <v>36</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="3" t="n">
         <v>5019</v>
       </c>
-      <c r="G45" s="9" t="s">
-        <v>127</v>
+      <c r="G45" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1</v>
@@ -1944,43 +2005,46 @@
         <f aca="false">B46*3</f>
         <v>3</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>145</v>
+      <c r="D46" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="0" t="n">
+      <c r="A47" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="C47" s="3" t="n">
         <f aca="false">B47*3</f>
-        <v>3</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="E47" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>150</v>
+      <c r="E47" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>5019</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1</v>
@@ -1989,19 +2053,19 @@
         <f aca="false">B48*3</f>
         <v>3</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1</v>
@@ -2011,18 +2075,21 @@
         <v>3</v>
       </c>
       <c r="D49" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="G49" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1</v>
@@ -2032,42 +2099,39 @@
         <v>3</v>
       </c>
       <c r="D50" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="F50" s="0" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="0" t="n">
         <f aca="false">B51*3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D51" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="F51" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1</v>
@@ -2077,15 +2141,12 @@
         <v>3</v>
       </c>
       <c r="D52" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="F52" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="G52" s="0" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2094,11 +2155,11 @@
         <v>170</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53" s="0" t="n">
         <f aca="false">B53*3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>171</v>
@@ -2107,6 +2168,9 @@
         <v>172</v>
       </c>
       <c r="F53" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" s="0" t="s">
         <v>173</v>
       </c>
     </row>
@@ -2125,36 +2189,81 @@
         <v>175</v>
       </c>
       <c r="E54" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G54" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" s="0" t="n">
         <f aca="false">B55*3</f>
+        <v>3</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <f aca="false">B56*3</f>
+        <v>3</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <f aca="false">B57*3</f>
         <v>9</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F55" s="0" t="s">
-        <v>181</v>
+      <c r="D57" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" display="A98333-ND"/>
+    <hyperlink ref="F12" r:id="rId1" display="A98333-ND "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Finished initial component placement
</commit_message>
<xml_diff>
--- a/Hardware/Three_Phase_Inverter_Controller.xlsx
+++ b/Hardware/Three_Phase_Inverter_Controller.xlsx
@@ -388,7 +388,7 @@
     <t xml:space="preserve">RNCP0805FTD10R0</t>
   </si>
   <si>
-    <t xml:space="preserve">R10 R11 R19 R2 R23 R27 R28 R3 R31 R32 R39 R4 R40 R41 R42 R43 R44 R46 R5 R6 R7 R8 R9 </t>
+    <t xml:space="preserve">R10 R11 R19 R2 R23 R27 R28 R3 R31 R32 R47 R4 R40 R41 R42 R43 R44 R46 R5 R6 R7 R8 R9 </t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -985,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>